<commit_message>
ajuste na planilha sinapi e info de build
</commit_message>
<xml_diff>
--- a/app/static/planilha_base_orcamento_sinapi.xlsx
+++ b/app/static/planilha_base_orcamento_sinapi.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="6780"/>
+    <workbookView windowWidth="20130" windowHeight="8085"/>
   </bookViews>
   <sheets>
     <sheet name="Lista de Orçamento Sinapi" sheetId="1" r:id="rId1"/>
@@ -1284,7 +1284,7 @@
     <numFmt numFmtId="180" formatCode="&quot;R$&quot;\ #,##0.00"/>
     <numFmt numFmtId="181" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="44">
+  <fonts count="43">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1379,12 +1379,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -1931,158 +1925,158 @@
   </borders>
   <cellStyleXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="7" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="40" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="42" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="43" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="41" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2237,16 +2231,16 @@
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="15" fillId="0" borderId="0" xfId="53" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2263,16 +2257,16 @@
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" xfId="58" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="16" fillId="0" borderId="0" xfId="58" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="10" fontId="10" fillId="3" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2295,7 +2289,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -2305,7 +2299,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -2324,7 +2318,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2353,46 +2347,46 @@
     <xf numFmtId="181" fontId="5" fillId="3" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="1" xfId="53" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="53" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="53" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="21" fillId="2" borderId="0" xfId="58" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="21" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="20" fillId="2" borderId="0" xfId="58" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="20" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="53" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="53" applyFont="1"/>
+    <xf numFmtId="181" fontId="19" fillId="3" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="181" fontId="20" fillId="3" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="181" fontId="21" fillId="3" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="21" fillId="3" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="20" fillId="3" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="181" fontId="21" fillId="3" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="20" fillId="3" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="21" fillId="3" borderId="0" xfId="58" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="21" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="20" fillId="3" borderId="0" xfId="58" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="20" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="20" fillId="2" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="20" fillId="3" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="19" fillId="2" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="19" fillId="3" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="53" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="181" fontId="20" fillId="3" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="19" fillId="3" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="181" fontId="9" fillId="3" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2404,7 +2398,7 @@
     <xf numFmtId="181" fontId="9" fillId="3" borderId="0" xfId="50" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2417,7 +2411,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="19" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="18" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2788,7 +2782,7 @@
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="H687" sqref="H687"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2919,10 +2913,7 @@
       <c r="E8" s="34"/>
       <c r="F8" s="35"/>
       <c r="G8" s="35"/>
-      <c r="H8" s="36">
-        <f>SUM(H9,H32)</f>
-        <v>0</v>
-      </c>
+      <c r="H8" s="36"/>
       <c r="I8" s="63"/>
     </row>
     <row r="9" spans="1:9">
@@ -2935,10 +2926,7 @@
       <c r="E9" s="40"/>
       <c r="F9" s="41"/>
       <c r="G9" s="41"/>
-      <c r="H9" s="42">
-        <f>SUM(H10:H31)</f>
-        <v>0</v>
-      </c>
+      <c r="H9" s="42"/>
       <c r="I9" s="64"/>
     </row>
     <row r="10" outlineLevel="1" spans="1:9">
@@ -3315,10 +3303,7 @@
       <c r="E32" s="40"/>
       <c r="F32" s="41"/>
       <c r="G32" s="41"/>
-      <c r="H32" s="42">
-        <f>SUM(H33:H44)</f>
-        <v>0</v>
-      </c>
+      <c r="H32" s="42"/>
       <c r="I32" s="64"/>
     </row>
     <row r="33" outlineLevel="1" spans="1:9">
@@ -3530,10 +3515,7 @@
       <c r="E45" s="34"/>
       <c r="F45" s="35"/>
       <c r="G45" s="35"/>
-      <c r="H45" s="36">
-        <f>SUM(H200,H175,H161,H135,H106,H81,H64,H46)</f>
-        <v>0</v>
-      </c>
+      <c r="H45" s="36"/>
       <c r="I45" s="63"/>
     </row>
     <row r="46" spans="1:9">
@@ -3546,10 +3528,7 @@
       <c r="E46" s="40"/>
       <c r="F46" s="41"/>
       <c r="G46" s="41"/>
-      <c r="H46" s="42">
-        <f>SUM(H47:H63)</f>
-        <v>0</v>
-      </c>
+      <c r="H46" s="42"/>
       <c r="I46" s="64"/>
     </row>
     <row r="47" ht="36" outlineLevel="1" spans="1:9">
@@ -3835,10 +3814,7 @@
       <c r="E64" s="40"/>
       <c r="F64" s="41"/>
       <c r="G64" s="41"/>
-      <c r="H64" s="42">
-        <f>SUM(H65:H80)</f>
-        <v>0</v>
-      </c>
+      <c r="H64" s="42"/>
       <c r="I64" s="64"/>
     </row>
     <row r="65" ht="36" outlineLevel="1" spans="2:9">
@@ -4113,10 +4089,7 @@
       <c r="E81" s="40"/>
       <c r="F81" s="41"/>
       <c r="G81" s="41"/>
-      <c r="H81" s="42">
-        <f>SUM(H82:H105)</f>
-        <v>0</v>
-      </c>
+      <c r="H81" s="42"/>
       <c r="I81" s="64"/>
     </row>
     <row r="82" ht="36" outlineLevel="1" spans="2:9">
@@ -4540,10 +4513,7 @@
       <c r="E106" s="40"/>
       <c r="F106" s="41"/>
       <c r="G106" s="41"/>
-      <c r="H106" s="42">
-        <f>SUM(H107:H134)</f>
-        <v>0</v>
-      </c>
+      <c r="H106" s="42"/>
       <c r="I106" s="64"/>
     </row>
     <row r="107" outlineLevel="1" spans="2:9">
@@ -4990,10 +4960,7 @@
       <c r="E135" s="40"/>
       <c r="F135" s="41"/>
       <c r="G135" s="41"/>
-      <c r="H135" s="42">
-        <f>SUM(H136:H160)</f>
-        <v>0</v>
-      </c>
+      <c r="H135" s="42"/>
       <c r="I135" s="64"/>
     </row>
     <row r="136" ht="24" outlineLevel="1" spans="2:9">
@@ -5437,10 +5404,7 @@
       <c r="E161" s="40"/>
       <c r="F161" s="41"/>
       <c r="G161" s="41"/>
-      <c r="H161" s="42">
-        <f>SUM(H162:H174)</f>
-        <v>0</v>
-      </c>
+      <c r="H161" s="42"/>
       <c r="I161" s="64"/>
     </row>
     <row r="162" ht="48" outlineLevel="1" spans="2:9">
@@ -5661,10 +5625,7 @@
       <c r="E175" s="40"/>
       <c r="F175" s="41"/>
       <c r="G175" s="41"/>
-      <c r="H175" s="42">
-        <f>SUM(H176:H199)</f>
-        <v>0</v>
-      </c>
+      <c r="H175" s="42"/>
       <c r="I175" s="64"/>
     </row>
     <row r="176" ht="24" outlineLevel="1" spans="2:9">
@@ -6091,10 +6052,7 @@
       <c r="E200" s="64"/>
       <c r="F200" s="64"/>
       <c r="G200" s="64"/>
-      <c r="H200" s="42">
-        <f>SUM(H201:H220)</f>
-        <v>0</v>
-      </c>
+      <c r="H200" s="42"/>
       <c r="I200" s="64"/>
     </row>
     <row r="201" outlineLevel="1" spans="2:9">
@@ -6433,10 +6391,7 @@
       <c r="E221" s="34"/>
       <c r="F221" s="35"/>
       <c r="G221" s="35"/>
-      <c r="H221" s="36">
-        <f>SUM(H238,H222)</f>
-        <v>0</v>
-      </c>
+      <c r="H221" s="36"/>
       <c r="I221" s="63"/>
     </row>
     <row r="222" spans="1:9">
@@ -6449,10 +6404,7 @@
       <c r="E222" s="40"/>
       <c r="F222" s="41"/>
       <c r="G222" s="41"/>
-      <c r="H222" s="42">
-        <f>SUM(H223:H237)</f>
-        <v>0</v>
-      </c>
+      <c r="H222" s="42"/>
       <c r="I222" s="64"/>
     </row>
     <row r="223" ht="36" outlineLevel="1" spans="1:9">
@@ -6715,10 +6667,7 @@
       <c r="E238" s="40"/>
       <c r="F238" s="41"/>
       <c r="G238" s="41"/>
-      <c r="H238" s="42">
-        <f>SUM(H239:H265)</f>
-        <v>0</v>
-      </c>
+      <c r="H238" s="42"/>
       <c r="I238" s="64"/>
     </row>
     <row r="239" ht="24" outlineLevel="1" spans="2:9">
@@ -7205,10 +7154,7 @@
       <c r="E266" s="40"/>
       <c r="F266" s="41"/>
       <c r="G266" s="41"/>
-      <c r="H266" s="42">
-        <f>SUM(H267:H290)</f>
-        <v>0</v>
-      </c>
+      <c r="H266" s="42"/>
       <c r="I266" s="64"/>
     </row>
     <row r="267" ht="24" outlineLevel="1" spans="3:9">
@@ -7619,10 +7565,7 @@
       <c r="E291" s="34"/>
       <c r="F291" s="35"/>
       <c r="G291" s="35"/>
-      <c r="H291" s="36">
-        <f>SUM(H313,H302,H292)</f>
-        <v>0</v>
-      </c>
+      <c r="H291" s="36"/>
       <c r="I291" s="63"/>
     </row>
     <row r="292" spans="2:9">
@@ -7634,10 +7577,7 @@
       <c r="E292" s="40"/>
       <c r="F292" s="41"/>
       <c r="G292" s="41"/>
-      <c r="H292" s="42">
-        <f>SUM(H293:H301)</f>
-        <v>0</v>
-      </c>
+      <c r="H292" s="42"/>
       <c r="I292" s="64"/>
     </row>
     <row r="293" ht="24" outlineLevel="1" spans="3:8">
@@ -7770,10 +7710,7 @@
       <c r="E302" s="40"/>
       <c r="F302" s="41"/>
       <c r="G302" s="41"/>
-      <c r="H302" s="42">
-        <f>SUM(H303:H312)</f>
-        <v>0</v>
-      </c>
+      <c r="H302" s="42"/>
       <c r="I302" s="64"/>
     </row>
     <row r="303" ht="36" outlineLevel="1" spans="3:8">
@@ -7917,10 +7854,7 @@
       <c r="E313" s="40"/>
       <c r="F313" s="41"/>
       <c r="G313" s="41"/>
-      <c r="H313" s="42">
-        <f>SUM(H314:H326)</f>
-        <v>0</v>
-      </c>
+      <c r="H313" s="42"/>
       <c r="I313" s="64"/>
     </row>
     <row r="314" ht="24" outlineLevel="1" spans="3:8">
@@ -8108,10 +8042,7 @@
       <c r="E327" s="34"/>
       <c r="F327" s="35"/>
       <c r="G327" s="35"/>
-      <c r="H327" s="36">
-        <f>SUM(H412,H399,H385,H356,H345,H328)</f>
-        <v>0</v>
-      </c>
+      <c r="H327" s="36"/>
       <c r="I327" s="63"/>
     </row>
     <row r="328" spans="2:9">
@@ -8123,10 +8054,7 @@
       <c r="E328" s="40"/>
       <c r="F328" s="41"/>
       <c r="G328" s="41"/>
-      <c r="H328" s="42">
-        <f>SUM(H329:H344)</f>
-        <v>0</v>
-      </c>
+      <c r="H328" s="42"/>
       <c r="I328" s="64"/>
     </row>
     <row r="329" ht="48" outlineLevel="1" spans="1:8">
@@ -8390,10 +8318,7 @@
       <c r="E345" s="40"/>
       <c r="F345" s="41"/>
       <c r="G345" s="41"/>
-      <c r="H345" s="42">
-        <f>SUM(H346:H355)</f>
-        <v>0</v>
-      </c>
+      <c r="H345" s="42"/>
       <c r="I345" s="64"/>
     </row>
     <row r="346" ht="36" outlineLevel="1" spans="1:8">
@@ -8555,10 +8480,7 @@
       <c r="E356" s="40"/>
       <c r="F356" s="41"/>
       <c r="G356" s="41"/>
-      <c r="H356" s="42">
-        <f>SUM(H357:H371)</f>
-        <v>0</v>
-      </c>
+      <c r="H356" s="42"/>
       <c r="I356" s="64"/>
     </row>
     <row r="357" ht="36" outlineLevel="1" spans="1:8">
@@ -8806,10 +8728,7 @@
       <c r="E372" s="34"/>
       <c r="F372" s="35"/>
       <c r="G372" s="35"/>
-      <c r="H372" s="36">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
+      <c r="H372" s="36"/>
       <c r="I372" s="63"/>
     </row>
     <row r="373" outlineLevel="1" spans="2:9">
@@ -8821,10 +8740,7 @@
       <c r="E373" s="40"/>
       <c r="F373" s="41"/>
       <c r="G373" s="41"/>
-      <c r="H373" s="42">
-        <f>SUM(H374:H384)</f>
-        <v>0</v>
-      </c>
+      <c r="H373" s="42"/>
       <c r="I373" s="64"/>
     </row>
     <row r="374" ht="60" outlineLevel="1" spans="3:8">
@@ -8995,10 +8911,7 @@
       <c r="E385" s="40"/>
       <c r="F385" s="41"/>
       <c r="G385" s="41"/>
-      <c r="H385" s="42">
-        <f>SUM(H386:H398)</f>
-        <v>0</v>
-      </c>
+      <c r="H385" s="42"/>
       <c r="I385" s="64"/>
     </row>
     <row r="386" ht="24" outlineLevel="1" spans="3:8">
@@ -9185,10 +9098,7 @@
       <c r="E399" s="40"/>
       <c r="F399" s="41"/>
       <c r="G399" s="41"/>
-      <c r="H399" s="42">
-        <f>SUM(H400:H411)</f>
-        <v>0</v>
-      </c>
+      <c r="H399" s="42"/>
       <c r="I399" s="64"/>
     </row>
     <row r="400" ht="24" outlineLevel="1" spans="3:8">
@@ -9360,10 +9270,7 @@
       <c r="E412" s="40"/>
       <c r="F412" s="41"/>
       <c r="G412" s="41"/>
-      <c r="H412" s="42">
-        <f>SUM(H413:H418)</f>
-        <v>0</v>
-      </c>
+      <c r="H412" s="42"/>
       <c r="I412" s="64"/>
     </row>
     <row r="413" outlineLevel="1" spans="3:8">
@@ -9440,10 +9347,7 @@
       <c r="E419" s="34"/>
       <c r="F419" s="35"/>
       <c r="G419" s="35"/>
-      <c r="H419" s="36">
-        <f>SUM(H438,H420)</f>
-        <v>0</v>
-      </c>
+      <c r="H419" s="36"/>
       <c r="I419" s="63"/>
     </row>
     <row r="420" spans="2:9">
@@ -9455,10 +9359,7 @@
       <c r="E420" s="40"/>
       <c r="F420" s="41"/>
       <c r="G420" s="41"/>
-      <c r="H420" s="42">
-        <f>SUM(H421:H437)</f>
-        <v>0</v>
-      </c>
+      <c r="H420" s="42"/>
       <c r="I420" s="64"/>
     </row>
     <row r="421" ht="36" outlineLevel="1" spans="3:8">
@@ -9705,10 +9606,7 @@
       <c r="E438" s="40"/>
       <c r="F438" s="41"/>
       <c r="G438" s="41"/>
-      <c r="H438" s="42">
-        <f>SUM(H439:H447)</f>
-        <v>0</v>
-      </c>
+      <c r="H438" s="42"/>
       <c r="I438" s="64"/>
     </row>
     <row r="439" ht="60" outlineLevel="1" spans="3:8">
@@ -9830,10 +9728,7 @@
       <c r="E448" s="34"/>
       <c r="F448" s="35"/>
       <c r="G448" s="35"/>
-      <c r="H448" s="36">
-        <f>SUM(H449)</f>
-        <v>0</v>
-      </c>
+      <c r="H448" s="36"/>
       <c r="I448" s="63"/>
     </row>
     <row r="449" spans="2:9">
@@ -9845,10 +9740,7 @@
       <c r="E449" s="40"/>
       <c r="F449" s="41"/>
       <c r="G449" s="41"/>
-      <c r="H449" s="42">
-        <f>SUM(H450:H468)</f>
-        <v>0</v>
-      </c>
+      <c r="H449" s="42"/>
       <c r="I449" s="64"/>
     </row>
     <row r="450" ht="36" outlineLevel="1" spans="2:8">
@@ -10121,10 +10013,7 @@
       <c r="E469" s="34"/>
       <c r="F469" s="35"/>
       <c r="G469" s="35"/>
-      <c r="H469" s="36">
-        <f>SUM(H509,H501,H491,H482,H470)</f>
-        <v>0</v>
-      </c>
+      <c r="H469" s="36"/>
       <c r="I469" s="63"/>
     </row>
     <row r="470" spans="2:9">
@@ -10136,10 +10025,7 @@
       <c r="E470" s="40"/>
       <c r="F470" s="41"/>
       <c r="G470" s="41"/>
-      <c r="H470" s="42">
-        <f>SUM(H471:H481)</f>
-        <v>0</v>
-      </c>
+      <c r="H470" s="42"/>
       <c r="I470" s="64"/>
     </row>
     <row r="471" ht="24" outlineLevel="1" spans="3:8">
@@ -10290,10 +10176,7 @@
       <c r="E482" s="40"/>
       <c r="F482" s="41"/>
       <c r="G482" s="41"/>
-      <c r="H482" s="42">
-        <f>SUM(H483:H490)</f>
-        <v>0</v>
-      </c>
+      <c r="H482" s="42"/>
       <c r="I482" s="64"/>
     </row>
     <row r="483" ht="24" outlineLevel="1" spans="3:8">
@@ -10399,10 +10282,7 @@
       <c r="E491" s="40"/>
       <c r="F491" s="41"/>
       <c r="G491" s="41"/>
-      <c r="H491" s="42">
-        <f>SUM(H492:H500)</f>
-        <v>0</v>
-      </c>
+      <c r="H491" s="42"/>
       <c r="I491" s="64"/>
     </row>
     <row r="492" ht="36" outlineLevel="1" spans="3:8">
@@ -10523,10 +10403,7 @@
       <c r="E501" s="40"/>
       <c r="F501" s="41"/>
       <c r="G501" s="41"/>
-      <c r="H501" s="42">
-        <f>SUM(H502:H508)</f>
-        <v>0</v>
-      </c>
+      <c r="H501" s="42"/>
       <c r="I501" s="64"/>
     </row>
     <row r="502" outlineLevel="1" spans="3:8">
@@ -10615,10 +10492,7 @@
       <c r="E509" s="40"/>
       <c r="F509" s="41"/>
       <c r="G509" s="41"/>
-      <c r="H509" s="42">
-        <f>SUM(H510:H517)</f>
-        <v>0</v>
-      </c>
+      <c r="H509" s="42"/>
       <c r="I509" s="64"/>
     </row>
     <row r="510" ht="36" outlineLevel="1" spans="3:8">
@@ -10725,10 +10599,7 @@
       <c r="E518" s="34"/>
       <c r="F518" s="35"/>
       <c r="G518" s="35"/>
-      <c r="H518" s="36">
-        <f>SUM(H543,H519)</f>
-        <v>0</v>
-      </c>
+      <c r="H518" s="36"/>
       <c r="I518" s="63"/>
     </row>
     <row r="519" spans="2:9">
@@ -10740,10 +10611,7 @@
       <c r="E519" s="40"/>
       <c r="F519" s="41"/>
       <c r="G519" s="41"/>
-      <c r="H519" s="42">
-        <f>SUM(H520:H542)</f>
-        <v>0</v>
-      </c>
+      <c r="H519" s="42"/>
       <c r="I519" s="64"/>
     </row>
     <row r="520" ht="24" outlineLevel="1" spans="3:8">
@@ -11074,10 +10942,7 @@
       <c r="E543" s="40"/>
       <c r="F543" s="41"/>
       <c r="G543" s="41"/>
-      <c r="H543" s="42">
-        <f>SUM(H544:H553)</f>
-        <v>0</v>
-      </c>
+      <c r="H543" s="42"/>
       <c r="I543" s="64"/>
     </row>
     <row r="544" ht="36" outlineLevel="1" spans="2:8">
@@ -11215,10 +11080,7 @@
       <c r="E554" s="34"/>
       <c r="F554" s="35"/>
       <c r="G554" s="35"/>
-      <c r="H554" s="36">
-        <f>SUM(H555)</f>
-        <v>0</v>
-      </c>
+      <c r="H554" s="36"/>
       <c r="I554" s="63"/>
     </row>
     <row r="555" spans="2:9">
@@ -11230,10 +11092,7 @@
       <c r="E555" s="40"/>
       <c r="F555" s="41"/>
       <c r="G555" s="41"/>
-      <c r="H555" s="42">
-        <f>SUM(H556:H568)</f>
-        <v>0</v>
-      </c>
+      <c r="H555" s="42"/>
       <c r="I555" s="64"/>
     </row>
     <row r="556" ht="24" outlineLevel="1" spans="3:8">
@@ -11415,10 +11274,7 @@
       <c r="E569" s="34"/>
       <c r="F569" s="35"/>
       <c r="G569" s="35"/>
-      <c r="H569" s="36">
-        <f>SUM(H570)</f>
-        <v>0</v>
-      </c>
+      <c r="H569" s="36"/>
       <c r="I569" s="63"/>
     </row>
     <row r="570" spans="2:9">
@@ -11430,10 +11286,7 @@
       <c r="E570" s="40"/>
       <c r="F570" s="41"/>
       <c r="G570" s="41"/>
-      <c r="H570" s="42">
-        <f>SUM(H571:H582)</f>
-        <v>0</v>
-      </c>
+      <c r="H570" s="42"/>
       <c r="I570" s="64"/>
     </row>
     <row r="571" ht="36" outlineLevel="1" spans="3:8">
@@ -11600,10 +11453,7 @@
       <c r="E583" s="34"/>
       <c r="F583" s="35"/>
       <c r="G583" s="35"/>
-      <c r="H583" s="36">
-        <f>SUM(H604,H593,H584)</f>
-        <v>0</v>
-      </c>
+      <c r="H583" s="36"/>
       <c r="I583" s="63"/>
     </row>
     <row r="584" spans="2:9">
@@ -11615,10 +11465,7 @@
       <c r="E584" s="40"/>
       <c r="F584" s="41"/>
       <c r="G584" s="41"/>
-      <c r="H584" s="42">
-        <f>SUM(H585:H592)</f>
-        <v>0</v>
-      </c>
+      <c r="H584" s="42"/>
       <c r="I584" s="64"/>
     </row>
     <row r="585" ht="48" outlineLevel="1" spans="2:8">
@@ -11730,10 +11577,7 @@
       <c r="E593" s="40"/>
       <c r="F593" s="41"/>
       <c r="G593" s="41"/>
-      <c r="H593" s="42">
-        <f>SUM(H594:H603)</f>
-        <v>0</v>
-      </c>
+      <c r="H593" s="42"/>
       <c r="I593" s="64"/>
     </row>
     <row r="594" outlineLevel="1" spans="2:8">
@@ -11870,10 +11714,7 @@
       <c r="E604" s="101"/>
       <c r="F604" s="41"/>
       <c r="G604" s="41"/>
-      <c r="H604" s="42">
-        <f>SUM(H605:H612)</f>
-        <v>0</v>
-      </c>
+      <c r="H604" s="42"/>
       <c r="I604" s="64"/>
     </row>
     <row r="605" outlineLevel="1" spans="2:8">
@@ -11976,10 +11817,7 @@
       <c r="E613" s="106"/>
       <c r="F613" s="107"/>
       <c r="G613" s="107"/>
-      <c r="H613" s="108">
-        <f>SUM(H638,H614)</f>
-        <v>0</v>
-      </c>
+      <c r="H613" s="108"/>
       <c r="I613" s="116"/>
     </row>
     <row r="614" s="2" customFormat="1" spans="1:9">
@@ -11992,10 +11830,7 @@
       <c r="E614" s="113"/>
       <c r="F614" s="114"/>
       <c r="G614" s="114"/>
-      <c r="H614" s="115">
-        <f>SUM(H615:H637)</f>
-        <v>0</v>
-      </c>
+      <c r="H614" s="115"/>
       <c r="I614" s="117"/>
     </row>
     <row r="615" ht="24" outlineLevel="1" spans="3:8">
@@ -12349,10 +12184,7 @@
       <c r="E638" s="113"/>
       <c r="F638" s="114"/>
       <c r="G638" s="114"/>
-      <c r="H638" s="115">
-        <f>SUM(H639:H649)</f>
-        <v>0</v>
-      </c>
+      <c r="H638" s="115"/>
       <c r="I638" s="117"/>
     </row>
     <row r="639" ht="24" outlineLevel="1" spans="3:8">
@@ -12512,10 +12344,7 @@
       <c r="E650" s="34"/>
       <c r="F650" s="35"/>
       <c r="G650" s="35"/>
-      <c r="H650" s="36">
-        <f>SUM(H673,H663,H651)</f>
-        <v>0</v>
-      </c>
+      <c r="H650" s="36"/>
       <c r="I650" s="63"/>
     </row>
     <row r="651" spans="1:9">
@@ -12528,10 +12357,7 @@
       <c r="E651" s="40"/>
       <c r="F651" s="41"/>
       <c r="G651" s="41"/>
-      <c r="H651" s="42">
-        <f>SUM(H652:H662)</f>
-        <v>0</v>
-      </c>
+      <c r="H651" s="42"/>
       <c r="I651" s="64"/>
     </row>
     <row r="652" outlineLevel="1" spans="2:8">
@@ -12694,10 +12520,7 @@
       <c r="E663" s="40"/>
       <c r="F663" s="41"/>
       <c r="G663" s="41"/>
-      <c r="H663" s="42">
-        <f>SUM(H664:H672)</f>
-        <v>0</v>
-      </c>
+      <c r="H663" s="42"/>
       <c r="I663" s="64"/>
     </row>
     <row r="664" outlineLevel="1" spans="2:8">
@@ -12822,10 +12645,7 @@
       <c r="E673" s="40"/>
       <c r="F673" s="41"/>
       <c r="G673" s="41"/>
-      <c r="H673" s="42">
-        <f>SUM(H674:H683)</f>
-        <v>0</v>
-      </c>
+      <c r="H673" s="42"/>
       <c r="I673" s="64"/>
     </row>
     <row r="674" ht="36" outlineLevel="1" spans="2:8">

</xml_diff>

<commit_message>
ajustes grafico valor e sinapi
</commit_message>
<xml_diff>
--- a/app/static/planilha_base_orcamento_sinapi.xlsx
+++ b/app/static/planilha_base_orcamento_sinapi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Projetos\my\GFCnew\app\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95177D1B-6930-4E78-9A82-02116D366FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34560D0-BD2C-4B32-B29D-9B16B999F28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,17 +57,17 @@
     <t>Unid</t>
   </si>
   <si>
-    <t>Quant</t>
-  </si>
-  <si>
-    <t>Custo unit</t>
-  </si>
-  <si>
     <t>Cliente</t>
   </si>
   <si>
     <t>Quant
 Eng (França Part.)</t>
+  </si>
+  <si>
+    <t>Custo unit (Construtora)</t>
+  </si>
+  <si>
+    <t>Quant  (Construtora)</t>
   </si>
 </sst>
 </file>
@@ -921,7 +921,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -945,7 +945,7 @@
       <c r="A1" s="30"/>
       <c r="B1" s="22"/>
       <c r="C1" s="32" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="33"/>
       <c r="E1" s="48" t="s">
@@ -1032,13 +1032,13 @@
         <v>5</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H6" s="44" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>

</xml_diff>